<commit_message>
MA_07_02_C0 - Inserción digitación
Inserción del material recibido de digitación, se ajustó el guión y
faltan tres recursos por ajustar. El material de ilustración no se ha
recibido desde que se enviaron las observaciones de los ajustes.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/EsqueletoGuion_MA_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/EsqueletoGuion_MA_07_02_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Repositorio_MA_07\MA_07_02_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="13125" tabRatio="729" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1708,7 +1708,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,7 +2283,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2667,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>